<commit_message>
Anpassungen der Dokumente und Präsi
</commit_message>
<xml_diff>
--- a/Assets/Documents/Stanleys Abenteuer Aufgaben 22.01.2023.xlsx
+++ b/Assets/Documents/Stanleys Abenteuer Aufgaben 22.01.2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\GitHub\HangedLarryStan\Assets\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C2A688-D8CF-4AEC-96F8-DB3D4AF5C2DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745D2C0B-354E-4307-8532-D5311D4C859A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="56">
   <si>
     <t>Team 2</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Testing des Spiels: 7/10</t>
   </si>
   <si>
-    <t>Abschlusspräsentation: Texte und Implementierungsphasen, Qualitätssicherung, Abschluss und Ausblicke</t>
-  </si>
-  <si>
     <t>Gameplay Trailer: Die Teaserstory, die Funktionen, der Gegner und die Credits</t>
   </si>
   <si>
@@ -111,9 +108,6 @@
     <t>Phase 6: Qualitätssicherung</t>
   </si>
   <si>
-    <t>Aufgabenfeld im GitHub Projekt</t>
-  </si>
-  <si>
     <t>Bearbeiter</t>
   </si>
   <si>
@@ -132,9 +126,6 @@
     <t>Animationen und Bilder</t>
   </si>
   <si>
-    <t>Verteilung der neuen Funktion und des Gegners</t>
-  </si>
-  <si>
     <t>Lefti, Tony, Niran, Frank und Erik</t>
   </si>
   <si>
@@ -168,13 +159,41 @@
     <t>Wahrscheinlich PDF</t>
   </si>
   <si>
-    <t>Zur fehlerfreien Umsetzung des Gesamtspieles mit allen vom Game Design gewünschten Funktionen</t>
-  </si>
-  <si>
     <t>Lefti, Niran und Frank</t>
   </si>
   <si>
     <t>Fertig bis spätestens 20:30</t>
+  </si>
+  <si>
+    <t>Bewertungsteam</t>
+  </si>
+  <si>
+    <t>Game Art (25%)</t>
+  </si>
+  <si>
+    <t>Game Programmierung (25%)</t>
+  </si>
+  <si>
+    <t>Erstellung des Codes zur Umsetzung im Spiel</t>
+  </si>
+  <si>
+    <t>Game Design &amp;
+Präsentation (50%)</t>
+  </si>
+  <si>
+    <t>Verteilung der neuen Funktionen und des Gegners</t>
+  </si>
+  <si>
+    <t>Überarbeitung der Level 2 und 4 durch die neuen Funktionen</t>
+  </si>
+  <si>
+    <t>Fertigstellung der Abschlusspräsentation</t>
+  </si>
+  <si>
+    <t>Fertigstellung der fehlerfreien Umsetzung des  Spiels</t>
+  </si>
+  <si>
+    <t>Aufgabe im Projekt</t>
   </si>
 </sst>
 </file>
@@ -230,7 +249,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -378,17 +397,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -484,6 +492,58 @@
         <color indexed="64"/>
       </top>
       <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -492,7 +552,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -527,119 +587,131 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -921,341 +993,391 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:K26"/>
+  <dimension ref="A2:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="84.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="41.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="100.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="23.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="41.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="100.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E5" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="E6" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="6"/>
+      <c r="D8" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C9" s="6"/>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C10" s="6"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
-    </row>
-    <row r="11" spans="1:11" s="7" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B11" s="14" t="s">
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="1:12" s="7" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B11" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-    </row>
-    <row r="13" spans="1:11" s="4" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+    </row>
+    <row r="13" spans="1:12" s="4" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="L13" s="5"/>
+    </row>
+    <row r="14" spans="1:12" s="4" customFormat="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="L14" s="5"/>
+    </row>
+    <row r="15" spans="1:12" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="28"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="31"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="52"/>
+      <c r="L15" s="5"/>
+    </row>
+    <row r="16" spans="1:12" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="28"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="31"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="52"/>
+      <c r="L16" s="5"/>
+    </row>
+    <row r="17" spans="1:12" s="4" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="28"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="31"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="52"/>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="1:12" s="4" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="28"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="31"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="53"/>
+      <c r="L18" s="5"/>
+    </row>
+    <row r="19" spans="1:12" s="4" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="28"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="31"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="50" t="s">
+        <v>52</v>
+      </c>
+      <c r="L19" s="5"/>
+    </row>
+    <row r="20" spans="1:12" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="28"/>
+      <c r="B20" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="5" t="s">
+      <c r="C20" s="37"/>
+      <c r="D20" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="31"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="L20" s="5"/>
+    </row>
+    <row r="21" spans="1:12" s="4" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="29"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="32"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="L21" s="5"/>
+    </row>
+    <row r="22" spans="1:12" s="4" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="K13" s="5"/>
-    </row>
-    <row r="14" spans="1:11" s="4" customFormat="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="10" t="s">
+      <c r="C22" s="37"/>
+      <c r="D22" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="H22" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L22" s="5"/>
+    </row>
+    <row r="23" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="28"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="F23" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="K14" s="5"/>
-    </row>
-    <row r="15" spans="1:11" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="37"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="24"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="16"/>
-      <c r="K15" s="5"/>
-    </row>
-    <row r="16" spans="1:11" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="37"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="12" t="s">
+      <c r="G23" s="34"/>
+      <c r="H23" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="24"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="16"/>
-      <c r="K16" s="5"/>
-    </row>
-    <row r="17" spans="1:11" s="4" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="37"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E17" s="24"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="16"/>
-      <c r="K17" s="5"/>
-    </row>
-    <row r="18" spans="1:11" s="4" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="37"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="8" t="s">
+      <c r="I23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L23" s="5"/>
+    </row>
+    <row r="24" spans="1:12" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="29"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="24"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="19"/>
-      <c r="K18" s="5"/>
-    </row>
-    <row r="19" spans="1:11" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="37"/>
-      <c r="B19" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="24"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="K19" s="5"/>
-    </row>
-    <row r="20" spans="1:11" s="4" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="38"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="18"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="K20" s="5"/>
-    </row>
-    <row r="21" spans="1:11" s="4" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="26" t="s">
+      <c r="F24" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="G21" s="45" t="s">
-        <v>19</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K21" s="5"/>
-    </row>
-    <row r="22" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="37"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="43"/>
-      <c r="G22" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K22" s="5"/>
-    </row>
-    <row r="23" spans="1:11" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="38"/>
-      <c r="B23" s="44"/>
-      <c r="C23" s="46" t="s">
+      <c r="G24" s="35"/>
+      <c r="H24" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" s="48"/>
-      <c r="G23" s="49" t="s">
-        <v>18</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="K23" s="5"/>
-    </row>
-    <row r="24" spans="1:11" s="4" customFormat="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="27"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="32"/>
-      <c r="K24" s="5"/>
-    </row>
-    <row r="25" spans="1:11" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B25" s="27"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="32"/>
-      <c r="K25" s="5"/>
-    </row>
-    <row r="26" spans="1:11" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B26" s="27"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="32"/>
-      <c r="K26" s="5"/>
+      <c r="L24" s="5"/>
+    </row>
+    <row r="25" spans="1:12" s="4" customFormat="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="17"/>
+      <c r="L25" s="5"/>
+    </row>
+    <row r="26" spans="1:12" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="17"/>
+      <c r="L26" s="5"/>
+    </row>
+    <row r="27" spans="1:12" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="17"/>
+      <c r="L27" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A14:A20"/>
-    <mergeCell ref="E14:E20"/>
-    <mergeCell ref="G14:G18"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="F14:F20"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="B11:G11"/>
+  <mergeCells count="15">
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="C19:C24"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H14:H18"/>
+    <mergeCell ref="A14:A21"/>
+    <mergeCell ref="F14:F21"/>
+    <mergeCell ref="G22:G24"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="G14:G21"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="B20:B21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Präsentation und restliche Qualitätsanpassungadokumente
</commit_message>
<xml_diff>
--- a/Assets/Documents/Stanleys Abenteuer Aufgaben 22.01.2023.xlsx
+++ b/Assets/Documents/Stanleys Abenteuer Aufgaben 22.01.2023.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frank.Scheuer\Documents\GitHub\HangedLarryStan\Assets\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\GitHub\HangedLarryStan\Assets\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75180CF1-1046-4189-B99E-931943B66895}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E65D6D-0EC9-4BB6-925C-59FD42F91D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="56">
   <si>
     <t>Team 2</t>
   </si>
@@ -194,21 +194,6 @@
   </si>
   <si>
     <t>Bewertungskriterium</t>
-  </si>
-  <si>
-    <t>Krieg ich hin</t>
-  </si>
-  <si>
-    <t>Krieg ich nicht ohne Hardware hin</t>
-  </si>
-  <si>
-    <t>Krieg ich irgendwie hin</t>
-  </si>
-  <si>
-    <t>Mein Bereich</t>
-  </si>
-  <si>
-    <t>Krieg ich nicht hin</t>
   </si>
 </sst>
 </file>
@@ -573,7 +558,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -605,133 +590,145 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1017,7 +1014,7 @@
   <dimension ref="A2:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D18" sqref="D18:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,16 +1035,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -1056,11 +1053,11 @@
       <c r="D5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -1069,11 +1066,11 @@
       <c r="D6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -1099,15 +1096,15 @@
       <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:12" s="7" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
     </row>
     <row r="13" spans="1:12" s="4" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
@@ -1137,245 +1134,218 @@
       <c r="L13" s="5"/>
     </row>
     <row r="14" spans="1:12" s="4" customFormat="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="52" t="s">
+      <c r="D14" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="52" t="s">
+      <c r="E14" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="17" t="s">
+      <c r="G14" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="18" t="s">
+      <c r="H14" s="34" t="s">
         <v>32</v>
       </c>
       <c r="L14" s="5"/>
     </row>
     <row r="15" spans="1:12" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="53" t="s">
+      <c r="A15" s="38"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="53" t="s">
+      <c r="E15" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="21"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="23"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="35"/>
       <c r="L15" s="5"/>
     </row>
     <row r="16" spans="1:12" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="24" t="s">
+      <c r="A16" s="38"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="24" t="s">
+      <c r="E16" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="21"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="23"/>
-      <c r="J16" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="F16" s="41"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="35"/>
       <c r="L16" s="5"/>
     </row>
     <row r="17" spans="1:12" s="4" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="19"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="26" t="s">
+      <c r="A17" s="38"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="26" t="s">
+      <c r="E17" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="21"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="23"/>
-      <c r="J17" s="4" t="s">
-        <v>57</v>
-      </c>
+      <c r="F17" s="41"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="35"/>
       <c r="L17" s="5"/>
     </row>
     <row r="18" spans="1:12" s="4" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="19"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="27" t="s">
+      <c r="A18" s="38"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="E18" s="28" t="s">
+      <c r="E18" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="21"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="29"/>
-      <c r="J18" s="4" t="s">
-        <v>58</v>
-      </c>
+      <c r="F18" s="41"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="36"/>
       <c r="L18" s="5"/>
     </row>
     <row r="19" spans="1:12" s="4" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="19"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="30" t="s">
+      <c r="A19" s="38"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="31" t="s">
+      <c r="D19" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="21"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="32" t="s">
+      <c r="F19" s="41"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="J19" s="4" t="s">
-        <v>59</v>
-      </c>
       <c r="L19" s="5"/>
     </row>
     <row r="20" spans="1:12" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
-      <c r="B20" s="30" t="s">
+      <c r="A20" s="38"/>
+      <c r="B20" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="33" t="s">
+      <c r="C20" s="29"/>
+      <c r="D20" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="33" t="s">
+      <c r="E20" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="34" t="s">
+      <c r="F20" s="41"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="J20" s="4" t="s">
-        <v>59</v>
-      </c>
       <c r="L20" s="5"/>
     </row>
     <row r="21" spans="1:12" s="4" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="35"/>
-      <c r="B21" s="36"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="26" t="s">
+      <c r="A21" s="39"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="26" t="s">
+      <c r="E21" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="36"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="38" t="s">
+      <c r="F21" s="42"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="J21" s="4" t="s">
-        <v>58</v>
-      </c>
       <c r="L21" s="5"/>
     </row>
     <row r="22" spans="1:12" s="4" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="39" t="s">
+      <c r="B22" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="33" t="s">
+      <c r="C22" s="29"/>
+      <c r="D22" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E22" s="40" t="s">
+      <c r="E22" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="F22" s="41" t="s">
+      <c r="F22" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="42" t="s">
+      <c r="G22" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="H22" s="43" t="s">
+      <c r="H22" s="18" t="s">
         <v>18</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J22" s="4" t="s">
-        <v>60</v>
-      </c>
       <c r="L22" s="5"/>
     </row>
     <row r="23" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="44" t="s">
+      <c r="A23" s="38"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="E23" s="44" t="s">
+      <c r="E23" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F23" s="45" t="s">
+      <c r="F23" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="G23" s="46"/>
-      <c r="H23" s="43" t="s">
+      <c r="G23" s="44"/>
+      <c r="H23" s="18" t="s">
         <v>39</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J23" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="L23" s="5"/>
     </row>
     <row r="24" spans="1:12" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="35"/>
-      <c r="B24" s="47"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="48" t="s">
+      <c r="A24" s="39"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="E24" s="48" t="s">
+      <c r="E24" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="F24" s="49" t="s">
+      <c r="F24" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="G24" s="50"/>
-      <c r="H24" s="51" t="s">
+      <c r="G24" s="45"/>
+      <c r="H24" s="23" t="s">
         <v>52</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>56</v>
       </c>
       <c r="L24" s="5"/>
     </row>

</xml_diff>